<commit_message>
Add more api and rename folder
</commit_message>
<xml_diff>
--- a/docs/4_sprint_deliverables/Phase I/SprintBackLog - 1.xlsx
+++ b/docs/4_sprint_deliverables/Phase I/SprintBackLog - 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jr_Kns/Desktop/Works/SE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jr_Kns/git/mms-lottery-kitchen-v2/docs/4_sprint_deliverables/Phase I/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="2560" yWindow="320" windowWidth="20480" windowHeight="15360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Ascharapon</t>
-  </si>
-  <si>
-    <t>Actual</t>
   </si>
   <si>
     <t>Testing</t>
@@ -201,6 +198,9 @@
       </rPr>
       <t>[Given] that student know exactly what tutors they need.     [When] student what to search for tutor.                         [Then] Ensure the search results is correct.</t>
     </r>
+  </si>
+  <si>
+    <t>Estimate</t>
   </si>
 </sst>
 </file>
@@ -395,6 +395,36 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -412,36 +442,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,7 +517,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$15:$Y$15</c:f>
+              <c:f>Sheet1!$K$22:$Y$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -528,42 +528,27 @@
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -579,33 +564,33 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$16:$Y$16</c:f>
+              <c:f>Sheet1!$K$15:$Y$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>17.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
@@ -643,11 +628,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1533955568"/>
-        <c:axId val="1440627488"/>
+        <c:axId val="-2012835888"/>
+        <c:axId val="-2012832496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1533955568"/>
+        <c:axId val="-2012835888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,7 +668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1440627488"/>
+        <c:crossAx val="-2012832496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -691,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440627488"/>
+        <c:axId val="-2012832496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,7 +694,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Point</a:t>
+                  <a:t>Effort</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -721,7 +706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1533955568"/>
+        <c:crossAx val="-2012835888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1063,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1178,8 +1163,8 @@
       <c r="E3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>48</v>
+      <c r="F3" s="26" t="s">
+        <v>47</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>38</v>
@@ -1247,7 +1232,7 @@
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
-      <c r="F4" s="35"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="17" t="s">
         <v>39</v>
       </c>
@@ -1314,7 +1299,7 @@
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
-      <c r="F5" s="35"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="17" t="s">
         <v>40</v>
       </c>
@@ -1381,14 +1366,14 @@
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" s="26" t="s">
+      <c r="F6" s="27"/>
+      <c r="G6" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="38" t="s">
         <v>30</v>
       </c>
       <c r="J6" s="19">
@@ -1448,81 +1433,81 @@
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
-      <c r="V7" s="38"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="38"/>
-      <c r="Y7" s="38"/>
-      <c r="Z7" s="38"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
     </row>
     <row r="8" spans="2:26" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39"/>
-      <c r="W8" s="39"/>
-      <c r="X8" s="39"/>
-      <c r="Y8" s="39"/>
-      <c r="Z8" s="39"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="33"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="33"/>
     </row>
     <row r="9" spans="2:26" ht="200" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="40"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
-      <c r="Y9" s="40"/>
-      <c r="Z9" s="40"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
     </row>
     <row r="10" spans="2:26" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="16"/>
@@ -1553,7 +1538,7 @@
     </row>
     <row r="11" spans="2:26" ht="14" x14ac:dyDescent="0.15">
       <c r="F11" s="5"/>
-      <c r="G11" s="32"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="6"/>
       <c r="I11" s="11" t="s">
         <v>28</v>
@@ -1579,7 +1564,7 @@
     </row>
     <row r="12" spans="2:26" ht="14" x14ac:dyDescent="0.15">
       <c r="F12" s="5"/>
-      <c r="G12" s="32"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="6"/>
       <c r="I12" s="11" t="s">
         <v>30</v>
@@ -1605,7 +1590,7 @@
     </row>
     <row r="13" spans="2:26" ht="14" x14ac:dyDescent="0.15">
       <c r="F13" s="5"/>
-      <c r="G13" s="32"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="6"/>
       <c r="I13" s="11" t="s">
         <v>32</v>
@@ -1630,7 +1615,7 @@
       <c r="Y13" s="7"/>
     </row>
     <row r="14" spans="2:26" ht="14" x14ac:dyDescent="0.15">
-      <c r="G14" s="33"/>
+      <c r="G14" s="24"/>
       <c r="I14" s="11" t="s">
         <v>27</v>
       </c>
@@ -1711,92 +1696,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.15">
-      <c r="I16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="1">
-        <v>18</v>
-      </c>
-      <c r="K16" s="1">
-        <v>17</v>
-      </c>
-      <c r="L16" s="1">
-        <v>16</v>
-      </c>
-      <c r="M16" s="1">
-        <v>16</v>
-      </c>
-      <c r="N16" s="1">
-        <v>15</v>
-      </c>
-      <c r="O16" s="1">
-        <v>15</v>
-      </c>
-      <c r="P16" s="1">
-        <v>7</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>3</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1</v>
-      </c>
-      <c r="S16" s="1">
-        <v>0</v>
-      </c>
-      <c r="T16" s="1">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1">
-        <v>0</v>
-      </c>
-      <c r="V16" s="1">
-        <v>0</v>
-      </c>
-      <c r="W16" s="1">
-        <v>0</v>
-      </c>
-      <c r="X16" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="8:10" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="8:20" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H19" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="8:20" x14ac:dyDescent="0.15">
       <c r="H20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J22" s="37"/>
-    </row>
-    <row r="23" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J23" s="37"/>
-    </row>
-    <row r="24" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J24" s="37"/>
-    </row>
-    <row r="25" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J25" s="37"/>
-    </row>
-    <row r="26" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J26" s="37"/>
-    </row>
-    <row r="27" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J27" s="37"/>
-    </row>
-    <row r="28" spans="8:10" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J28" s="37"/>
-    </row>
-    <row r="29" spans="8:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="J29" s="37"/>
+    <row r="22" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="1">
+        <v>18</v>
+      </c>
+      <c r="L22" s="1">
+        <v>16</v>
+      </c>
+      <c r="M22" s="1">
+        <v>14</v>
+      </c>
+      <c r="N22" s="1">
+        <v>12</v>
+      </c>
+      <c r="O22" s="1">
+        <v>10</v>
+      </c>
+      <c r="P22" s="1">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>6</v>
+      </c>
+      <c r="R22" s="1">
+        <v>4</v>
+      </c>
+      <c r="S22" s="1">
+        <v>2</v>
+      </c>
+      <c r="T22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="25"/>
+    </row>
+    <row r="24" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="25"/>
+    </row>
+    <row r="25" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="25"/>
+    </row>
+    <row r="26" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="25"/>
+    </row>
+    <row r="27" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="25"/>
+    </row>
+    <row r="28" spans="8:20" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="25"/>
+    </row>
+    <row r="29" spans="8:20" ht="18" x14ac:dyDescent="0.2">
+      <c r="J29" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="25">

</xml_diff>